<commit_message>
small correction in gannt chart hypothetical
</commit_message>
<xml_diff>
--- a/GanntChartCodingGameEstimatesHypothetical.xlsx
+++ b/GanntChartCodingGameEstimatesHypothetical.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E039E02E-EC83-F94A-8C4C-5AA4BDEF069B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2A52E9-B4C8-A948-8684-77563CE6FD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,6 +803,18 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -810,18 +822,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1392,7 +1392,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1447,124 +1447,124 @@
       <c r="B3" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="69">
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="66">
         <f ca="1">TODAY()</f>
         <v>44599</v>
       </c>
-      <c r="H3" s="69"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="64"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="68"/>
       <c r="G4" s="7">
         <v>-1</v>
       </c>
-      <c r="K4" s="66">
+      <c r="K4" s="63">
         <f ca="1">K5</f>
         <v>44585</v>
       </c>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="66">
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="63">
         <f ca="1">R5</f>
         <v>44592</v>
       </c>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="67"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="66">
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
+      <c r="W4" s="64"/>
+      <c r="X4" s="65"/>
+      <c r="Y4" s="63">
         <f ca="1">Y5</f>
         <v>44599</v>
       </c>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
-      <c r="AB4" s="67"/>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="67"/>
-      <c r="AE4" s="68"/>
-      <c r="AF4" s="66">
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="64"/>
+      <c r="AC4" s="64"/>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="65"/>
+      <c r="AF4" s="63">
         <f ca="1">AF5</f>
         <v>44606</v>
       </c>
-      <c r="AG4" s="67"/>
-      <c r="AH4" s="67"/>
-      <c r="AI4" s="67"/>
-      <c r="AJ4" s="67"/>
-      <c r="AK4" s="67"/>
-      <c r="AL4" s="68"/>
-      <c r="AM4" s="66">
+      <c r="AG4" s="64"/>
+      <c r="AH4" s="64"/>
+      <c r="AI4" s="64"/>
+      <c r="AJ4" s="64"/>
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="65"/>
+      <c r="AM4" s="63">
         <f ca="1">AM5</f>
         <v>44613</v>
       </c>
-      <c r="AN4" s="67"/>
-      <c r="AO4" s="67"/>
-      <c r="AP4" s="67"/>
-      <c r="AQ4" s="67"/>
-      <c r="AR4" s="67"/>
-      <c r="AS4" s="68"/>
-      <c r="AT4" s="66">
+      <c r="AN4" s="64"/>
+      <c r="AO4" s="64"/>
+      <c r="AP4" s="64"/>
+      <c r="AQ4" s="64"/>
+      <c r="AR4" s="64"/>
+      <c r="AS4" s="65"/>
+      <c r="AT4" s="63">
         <f ca="1">AT5</f>
         <v>44620</v>
       </c>
-      <c r="AU4" s="67"/>
-      <c r="AV4" s="67"/>
-      <c r="AW4" s="67"/>
-      <c r="AX4" s="67"/>
-      <c r="AY4" s="67"/>
-      <c r="AZ4" s="68"/>
-      <c r="BA4" s="66">
+      <c r="AU4" s="64"/>
+      <c r="AV4" s="64"/>
+      <c r="AW4" s="64"/>
+      <c r="AX4" s="64"/>
+      <c r="AY4" s="64"/>
+      <c r="AZ4" s="65"/>
+      <c r="BA4" s="63">
         <f ca="1">BA5</f>
         <v>44627</v>
       </c>
-      <c r="BB4" s="67"/>
-      <c r="BC4" s="67"/>
-      <c r="BD4" s="67"/>
-      <c r="BE4" s="67"/>
-      <c r="BF4" s="67"/>
-      <c r="BG4" s="68"/>
-      <c r="BH4" s="66">
+      <c r="BB4" s="64"/>
+      <c r="BC4" s="64"/>
+      <c r="BD4" s="64"/>
+      <c r="BE4" s="64"/>
+      <c r="BF4" s="64"/>
+      <c r="BG4" s="65"/>
+      <c r="BH4" s="63">
         <f ca="1">BH5</f>
         <v>44634</v>
       </c>
-      <c r="BI4" s="67"/>
-      <c r="BJ4" s="67"/>
-      <c r="BK4" s="67"/>
-      <c r="BL4" s="67"/>
-      <c r="BM4" s="67"/>
-      <c r="BN4" s="68"/>
+      <c r="BI4" s="64"/>
+      <c r="BJ4" s="64"/>
+      <c r="BK4" s="64"/>
+      <c r="BL4" s="64"/>
+      <c r="BM4" s="64"/>
+      <c r="BN4" s="65"/>
     </row>
     <row r="5" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
       <c r="K5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44585</v>
@@ -2467,16 +2467,16 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="55">
-        <v>44598</v>
+        <v>44597</v>
       </c>
       <c r="H12" s="55">
-        <f>G12+2</f>
+        <f>G12+3</f>
         <v>44600</v>
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="16">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K12" s="33"/>
       <c r="L12" s="33"/>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="E18" s="60"/>
       <c r="F18" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="56">
         <v>44596</v>
@@ -3051,16 +3051,16 @@
         <v>0.5</v>
       </c>
       <c r="G19" s="56">
-        <v>44598</v>
+        <v>44597</v>
       </c>
       <c r="H19" s="56">
-        <f>G19+2</f>
+        <f>G19+3</f>
         <v>44600</v>
       </c>
       <c r="I19" s="16"/>
       <c r="J19" s="16">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
@@ -3382,6 +3382,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="AT4:AZ4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BH4:BN4"/>
     <mergeCell ref="G3:H3"/>
@@ -3389,11 +3394,6 @@
     <mergeCell ref="R4:X4"/>
     <mergeCell ref="Y4:AE4"/>
     <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="AT4:AZ4"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F22">
     <cfRule type="dataBar" priority="14">

</xml_diff>